<commit_message>
Update Injector Lag for Bosch 0280155746
</commit_message>
<xml_diff>
--- a/Docs/Injectors Lag.xlsx
+++ b/Docs/Injectors Lag.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>ON</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>BMW 03762FA 180cc</t>
+  </si>
+  <si>
+    <t>Bosch 0280155746 200cc</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -145,6 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -446,48 +450,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>6</v>
       </c>
       <c r="B3" s="1">
@@ -510,9 +528,19 @@
         <f>E3-F3</f>
         <v>2.14</v>
       </c>
+      <c r="H3" s="1">
+        <v>2.71</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="J3" s="3">
+        <f>H3-I3</f>
+        <v>1.8599999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -535,9 +563,19 @@
         <f t="shared" ref="G4:G8" si="1">E4-F4</f>
         <v>1.2800000000000002</v>
       </c>
+      <c r="H4" s="1">
+        <v>1.93</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J8" si="2">H4-I4</f>
+        <v>1.08</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>10</v>
       </c>
       <c r="B5" s="1">
@@ -560,9 +598,19 @@
         <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
+      <c r="H5" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.77000000000000013</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>12</v>
       </c>
       <c r="B6" s="1">
@@ -585,9 +633,19 @@
         <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
+      <c r="H6" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.86</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46000000000000008</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>14</v>
       </c>
       <c r="B7" s="1">
@@ -610,9 +668,19 @@
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
+      <c r="H7" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.28999999999999992</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>16</v>
       </c>
       <c r="B8" s="4">
@@ -635,11 +703,22 @@
         <f t="shared" si="1"/>
         <v>0.16000000000000014</v>
       </c>
+      <c r="H8" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.88</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.10999999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add comment for different injector for 1.8l engine. Draft for 0280155968 420cc injectors
</commit_message>
<xml_diff>
--- a/Docs/Injectors Lag.xlsx
+++ b/Docs/Injectors Lag.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>ON</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Bosch 0280155746 200cc</t>
+  </si>
+  <si>
+    <t>Bosch 0280155968 420cc</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -149,6 +152,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -450,32 +456,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -503,8 +514,17 @@
       <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="K2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>6</v>
       </c>
@@ -538,8 +558,14 @@
         <f>H3-I3</f>
         <v>1.8599999999999999</v>
       </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3">
+        <f>K3-L3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>8</v>
       </c>
@@ -573,8 +599,14 @@
         <f t="shared" ref="J4:J8" si="2">H4-I4</f>
         <v>1.08</v>
       </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M8" si="3">K4-L4</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>10</v>
       </c>
@@ -608,8 +640,14 @@
         <f t="shared" si="2"/>
         <v>0.77000000000000013</v>
       </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>12</v>
       </c>
@@ -643,8 +681,14 @@
         <f t="shared" si="2"/>
         <v>0.46000000000000008</v>
       </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>14</v>
       </c>
@@ -678,8 +722,14 @@
         <f t="shared" si="2"/>
         <v>0.28999999999999992</v>
       </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>16</v>
       </c>
@@ -706,19 +756,26 @@
       <c r="H8" s="4">
         <v>0.99</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="5">
         <v>0.88</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="2"/>
         <v>0.10999999999999999</v>
       </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>